<commit_message>
logic update for userDB
</commit_message>
<xml_diff>
--- a/userDB.xlsx
+++ b/userDB.xlsx
@@ -423,10 +423,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5" outlineLevelCol="0"/>
@@ -492,6 +492,25 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>차니</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0x5a801efb2000003</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>

</xml_diff>